<commit_message>
cleaning up formatting in batch files
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/InitialisationFile.xlsx
+++ b/doc/Manual/Batchmode/InitialisationFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4528D57-FF27-4E32-8AA2-6D9212B03435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB89996-CA99-4444-93C5-0C97556C33B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11235" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description Cell-based" sheetId="1" r:id="rId1"/>
@@ -734,7 +734,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -837,15 +837,6 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -861,20 +852,40 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1310,7 +1321,7 @@
       <c r="C8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="38" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1324,7 +1335,7 @@
       <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="42"/>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
@@ -1336,7 +1347,7 @@
       <c r="C10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="42"/>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
@@ -1348,7 +1359,7 @@
       <c r="C11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="43"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
@@ -1472,7 +1483,7 @@
       <c r="C20" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="39" t="s">
+      <c r="D20" s="36" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1486,7 +1497,7 @@
       <c r="C21" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="40"/>
+      <c r="D21" s="37"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -6639,42 +6650,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="58" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="15.42578125" style="53" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="53" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.7109375" style="53" customWidth="1"/>
+    <col min="4" max="4" width="58" style="48" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="53"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="43" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="45" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -6684,307 +6695,307 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="25" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="44" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="45" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="45" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="46" t="s">
+      <c r="D8" s="38" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="47"/>
-    </row>
-    <row r="10" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="47"/>
-    </row>
-    <row r="11" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="48"/>
-    </row>
-    <row r="12" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
+      <c r="D11" s="40"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="29" t="s">
+      <c r="C13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="35" t="s">
+      <c r="D13" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="29" t="s">
+      <c r="C16" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D16" s="35" t="s">
+      <c r="D16" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="38" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="B18" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="36" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="34" t="s">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="36" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="34" t="s">
+    <row r="20" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="44" t="s">
+      <c r="D20" s="51" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="36" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="34" t="s">
+    <row r="21" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="50" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="45"/>
+      <c r="D21" s="52"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="12"/>
-      <c r="B22" s="12"/>
+      <c r="A22" s="48"/>
+      <c r="B22" s="48"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="12"/>
+      <c r="A23" s="48"/>
+      <c r="B23" s="48"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="12"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="12"/>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="12"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="48"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
-      <c r="B28" s="12"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="12"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="48"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="48"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="12"/>
-      <c r="B31" s="12"/>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="48"/>
+      <c r="B32" s="48"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
@@ -7023,50 +7034,50 @@
       <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
+      <c r="A39" s="48"/>
+      <c r="B39" s="48"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
+      <c r="A40" s="48"/>
+      <c r="B40" s="48"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="48"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="48"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="12"/>
-      <c r="B48" s="12"/>
+      <c r="A48" s="48"/>
+      <c r="B48" s="48"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="12"/>
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
@@ -7189,16 +7200,16 @@
       <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="12"/>
+      <c r="A70" s="48"/>
+      <c r="B70" s="48"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="12"/>
+      <c r="A71" s="48"/>
+      <c r="B71" s="48"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="12"/>
+      <c r="A72" s="48"/>
+      <c r="B72" s="48"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
@@ -7381,8 +7392,8 @@
       <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="12"/>
-      <c r="B103" s="12"/>
+      <c r="A103" s="48"/>
+      <c r="B103" s="48"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
@@ -7433,186 +7444,116 @@
       <c r="D111" s="15"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="12"/>
-      <c r="B112" s="12"/>
+      <c r="A112" s="48"/>
+      <c r="B112" s="48"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="12"/>
-      <c r="B113" s="12"/>
-      <c r="C113" s="12"/>
+      <c r="A113" s="48"/>
+      <c r="B113" s="48"/>
+      <c r="C113" s="48"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="12"/>
-      <c r="B114" s="12"/>
-      <c r="C114" s="12"/>
+      <c r="A114" s="48"/>
+      <c r="B114" s="48"/>
+      <c r="C114" s="48"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="12"/>
-      <c r="B115" s="12"/>
-      <c r="C115" s="12"/>
-      <c r="D115" s="6"/>
+      <c r="A115" s="48"/>
+      <c r="B115" s="48"/>
+      <c r="C115" s="48"/>
+      <c r="D115" s="53"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="12"/>
-      <c r="B116" s="12"/>
-      <c r="D116" s="6"/>
+      <c r="A116" s="48"/>
+      <c r="B116" s="48"/>
+      <c r="D116" s="53"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="12"/>
-      <c r="B117" s="12"/>
+      <c r="A117" s="48"/>
+      <c r="B117" s="48"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="12"/>
-      <c r="B118" s="12"/>
-      <c r="D118" s="6"/>
+      <c r="A118" s="48"/>
+      <c r="B118" s="48"/>
+      <c r="D118" s="53"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="12"/>
-      <c r="B119" s="12"/>
-      <c r="D119" s="6"/>
+      <c r="A119" s="48"/>
+      <c r="B119" s="48"/>
+      <c r="D119" s="53"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="12"/>
-      <c r="B120" s="12"/>
+      <c r="A120" s="48"/>
+      <c r="B120" s="48"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="12"/>
-      <c r="B121" s="12"/>
+      <c r="A121" s="48"/>
+      <c r="B121" s="48"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="12"/>
-      <c r="B122" s="12"/>
-      <c r="D122" s="6"/>
+      <c r="A122" s="48"/>
+      <c r="B122" s="48"/>
+      <c r="D122" s="53"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="12"/>
-      <c r="B123" s="12"/>
-      <c r="D123" s="6"/>
+      <c r="A123" s="48"/>
+      <c r="B123" s="48"/>
+      <c r="D123" s="53"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="12"/>
-      <c r="B124" s="12"/>
-      <c r="D124" s="6"/>
+      <c r="A124" s="48"/>
+      <c r="B124" s="48"/>
+      <c r="D124" s="53"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="12"/>
-      <c r="B125" s="12"/>
-      <c r="D125" s="6"/>
+      <c r="A125" s="48"/>
+      <c r="B125" s="48"/>
+      <c r="D125" s="53"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="6"/>
+      <c r="D126" s="53"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="6"/>
+      <c r="D127" s="53"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="6"/>
-    </row>
-    <row r="129" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D129" s="6"/>
-    </row>
-    <row r="130" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="6"/>
-    </row>
-    <row r="131" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="6"/>
-    </row>
-    <row r="132" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D132" s="6"/>
-    </row>
-    <row r="133" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D133" s="6"/>
-    </row>
-    <row r="134" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D134" s="6"/>
-    </row>
-    <row r="135" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D135" s="6"/>
-    </row>
-    <row r="136" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D136" s="6"/>
-    </row>
-    <row r="137" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="6"/>
-    </row>
-    <row r="138" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D138" s="6"/>
-    </row>
-    <row r="139" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D139" s="6"/>
-    </row>
-    <row r="140" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D140" s="6"/>
-    </row>
-    <row r="141" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D141" s="6"/>
-    </row>
-    <row r="142" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="6"/>
-    </row>
-    <row r="143" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="6"/>
-    </row>
-    <row r="144" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D144" s="6"/>
-    </row>
-    <row r="145" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D145" s="6"/>
-    </row>
-    <row r="146" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D146" s="6"/>
-    </row>
-    <row r="147" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D147" s="6"/>
-    </row>
-    <row r="148" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D148" s="6"/>
-    </row>
-    <row r="149" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D149" s="6"/>
-    </row>
-    <row r="150" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D150" s="6"/>
-    </row>
-    <row r="151" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D151" s="6"/>
-    </row>
-    <row r="152" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D152" s="6"/>
-    </row>
-    <row r="153" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D153" s="6"/>
-    </row>
-    <row r="154" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D154" s="6"/>
-    </row>
-    <row r="155" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D155" s="6"/>
-    </row>
-    <row r="156" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D156" s="6"/>
-    </row>
-    <row r="157" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D157" s="6"/>
-    </row>
-    <row r="158" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D158" s="6"/>
-    </row>
-    <row r="159" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D159" s="6"/>
-    </row>
-    <row r="160" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D160" s="6"/>
-    </row>
-    <row r="161" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D161" s="6"/>
-    </row>
-    <row r="162" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D162" s="6"/>
-    </row>
-    <row r="163" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D163" s="6"/>
-    </row>
+      <c r="D128" s="53"/>
+    </row>
+    <row r="129" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D20:D21"/>
@@ -7630,7 +7571,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7654,320 +7595,320 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="41" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="A2" s="42">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42">
+        <v>0</v>
+      </c>
+      <c r="C2" s="42">
+        <v>0</v>
+      </c>
+      <c r="D2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E2" s="42">
+        <v>0</v>
+      </c>
+      <c r="F2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0</v>
+      </c>
+      <c r="H2" s="42">
         <v>200</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="42">
+        <v>0</v>
+      </c>
+      <c r="J2" s="42">
         <v>200</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="42">
         <v>60</v>
       </c>
-      <c r="L2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="L2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M2" s="42">
+        <v>0</v>
+      </c>
+      <c r="N2" s="42">
+        <v>0</v>
+      </c>
+      <c r="O2" s="42">
+        <v>0</v>
+      </c>
+      <c r="P2" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
+      <c r="A3" s="42">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42">
+        <v>0</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+      <c r="D3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E3" s="42">
+        <v>2</v>
+      </c>
+      <c r="F3" s="42">
         <v>10.55</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="42">
+        <v>0</v>
+      </c>
+      <c r="H3" s="42">
         <v>200</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="42">
+        <v>0</v>
+      </c>
+      <c r="J3" s="42">
         <v>200</v>
       </c>
-      <c r="K3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M3">
+      <c r="K3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M3" s="42">
         <v>25</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="42">
         <v>30</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="42">
         <v>20</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="42">
         <v>150</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="C4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42">
+        <v>2</v>
+      </c>
+      <c r="F4" s="42">
         <v>17.2</v>
       </c>
-      <c r="G4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="G4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q4" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="42">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L5">
+      <c r="B5" s="42">
+        <v>1</v>
+      </c>
+      <c r="C5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D5" s="42">
+        <v>1</v>
+      </c>
+      <c r="E5" s="42">
+        <v>1</v>
+      </c>
+      <c r="F5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L5" s="42">
         <v>25</v>
       </c>
-      <c r="M5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="M5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q5" s="42" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="B6" s="42">
+        <v>2</v>
+      </c>
+      <c r="C6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="F6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q6" s="42" t="s">
         <v>78</v>
       </c>
     </row>
@@ -7981,10 +7922,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A1:U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8011,392 +7952,392 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="41" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
+      <c r="A2" s="42">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42">
+        <v>0</v>
+      </c>
+      <c r="C2" s="42">
+        <v>0</v>
+      </c>
+      <c r="D2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E2" s="42">
+        <v>0</v>
+      </c>
+      <c r="F2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G2" s="42">
+        <v>0</v>
+      </c>
+      <c r="H2" s="42">
         <v>200</v>
       </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-      <c r="J2">
+      <c r="I2" s="42">
+        <v>0</v>
+      </c>
+      <c r="J2" s="42">
         <v>200</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="42">
         <v>60</v>
       </c>
-      <c r="L2" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="L2" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M2" s="42">
+        <v>0</v>
+      </c>
+      <c r="N2" s="42">
+        <v>0</v>
+      </c>
+      <c r="O2" s="42">
+        <v>0</v>
+      </c>
+      <c r="P2" s="42">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
+      <c r="R2" s="42">
+        <v>0</v>
+      </c>
+      <c r="S2" s="42">
         <v>0.1</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="42">
         <v>0.3</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="42">
         <v>0.6</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
+      <c r="A3" s="42">
+        <v>2</v>
+      </c>
+      <c r="B3" s="42">
+        <v>0</v>
+      </c>
+      <c r="C3" s="42">
+        <v>1</v>
+      </c>
+      <c r="D3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E3" s="42">
+        <v>2</v>
+      </c>
+      <c r="F3" s="42">
         <v>10.55</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G3" s="42">
+        <v>0</v>
+      </c>
+      <c r="H3" s="42">
         <v>200</v>
       </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
+      <c r="I3" s="42">
+        <v>0</v>
+      </c>
+      <c r="J3" s="42">
         <v>200</v>
       </c>
-      <c r="K3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L3" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M3">
+      <c r="K3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L3" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M3" s="42">
         <v>25</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="42">
         <v>30</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="42">
         <v>20</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="42">
         <v>150</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="Q3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
+      <c r="R3" s="42">
+        <v>0</v>
+      </c>
+      <c r="S3" s="42">
+        <v>1</v>
+      </c>
+      <c r="T3" s="42">
+        <v>0</v>
+      </c>
+      <c r="U3" s="42">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="42">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
+      <c r="B4" s="42">
+        <v>1</v>
+      </c>
+      <c r="C4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D4" s="42">
+        <v>0</v>
+      </c>
+      <c r="E4" s="42">
+        <v>2</v>
+      </c>
+      <c r="F4" s="42">
         <v>17.2</v>
       </c>
-      <c r="G4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P4" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="G4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P4" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q4" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="R4">
-        <v>1</v>
-      </c>
-      <c r="S4">
+      <c r="R4" s="42">
+        <v>1</v>
+      </c>
+      <c r="S4" s="42">
         <v>0.2</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="42">
         <v>0.3</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="42">
         <v>0.5</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="42">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L5">
+      <c r="B5" s="42">
+        <v>1</v>
+      </c>
+      <c r="C5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D5" s="42">
+        <v>1</v>
+      </c>
+      <c r="E5" s="42">
+        <v>1</v>
+      </c>
+      <c r="F5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L5" s="42">
         <v>25</v>
       </c>
-      <c r="M5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P5" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="M5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P5" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q5" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="R5">
-        <v>2</v>
-      </c>
-      <c r="S5">
+      <c r="R5" s="42">
+        <v>2</v>
+      </c>
+      <c r="S5" s="42">
         <v>0.33300000000000002</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="42">
         <v>0.33300000000000002</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="42">
         <v>0.33400000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="42">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="D6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="E6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="F6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="H6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="I6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="J6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="K6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="L6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="M6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="N6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="O6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="P6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="B6" s="42">
+        <v>2</v>
+      </c>
+      <c r="C6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="D6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="E6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="F6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="G6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="H6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="I6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="J6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="K6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="L6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="M6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="N6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="O6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="P6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="Q6" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="R6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="S6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="T6" s="2">
-        <v>-9</v>
-      </c>
-      <c r="U6" s="2">
+      <c r="R6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="S6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="T6" s="42">
+        <v>-9</v>
+      </c>
+      <c r="U6" s="42">
         <v>-9</v>
       </c>
     </row>
@@ -8479,7 +8420,7 @@
       <c r="C4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="38" t="s">
         <v>69</v>
       </c>
     </row>
@@ -8493,7 +8434,7 @@
       <c r="C5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="43"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
@@ -9235,10 +9176,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
document that the origin is the bottom left corner
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/InitialisationFile.xlsx
+++ b/doc/Manual/Batchmode/InitialisationFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s02tp3\github\rs_batch_dev\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB89996-CA99-4444-93C5-0C97556C33B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186319D8-A922-495F-9503-D1458834EB7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11235" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="3450" windowWidth="21600" windowHeight="11235" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Description Cell-based" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="101">
   <si>
     <t>NOTES</t>
   </si>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>Must be &gt; 0 for patch-based model; if the patch does not exist in the landscape in the specified year, then the individual will not be initialised</t>
-  </si>
-  <si>
-    <t>Must be &gt;= 0 for cell-based model; if the specified cell (X,Y) lies beyond the landscape boundary, or is unsuitable in the specified year, then the individual will not be initialised</t>
   </si>
   <si>
     <t>Initial no. of individuals in each cell:  0 = at carrying capacity;  1 = at half carrying capacity;     2 = specified no. of individuals</t>
@@ -499,6 +496,12 @@
   </si>
   <si>
     <t>Type of initialisation from species distribution: 0 = All patches within the distribution cells,    1 = Some randomly chosen patches within distribution cells</t>
+  </si>
+  <si>
+    <t>Required for SeedType = 0 only; minX and minY may not be less than 0, maxX and maxY may not be less than corresponding minimum. The origin (0, 0) is the bottom -left corner.</t>
+  </si>
+  <si>
+    <t>Must be &gt;= 0 for cell-based model; if the specified cell (X,Y) lies beyond the landscape boundary, or is unsuitable in the specified year, then the individual will not be initialised. The origin (0, 0) is the bottom -left corner.</t>
   </si>
 </sst>
 </file>
@@ -734,7 +737,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -837,6 +840,15 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -851,41 +863,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1249,10 +1226,10 @@
         <v>18</v>
       </c>
       <c r="C3" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1291,10 +1268,10 @@
         <v>18</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1321,7 +1298,7 @@
       <c r="C8" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="D8" s="41" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1335,7 +1312,7 @@
       <c r="C9" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
@@ -1347,7 +1324,7 @@
       <c r="C10" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
@@ -1359,7 +1336,7 @@
       <c r="C11" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
@@ -1391,13 +1368,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>50</v>
@@ -1405,58 +1382,58 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>90</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B17" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>88</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="C18" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="D18" s="23" t="s">
         <v>75</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1483,8 +1460,8 @@
       <c r="C20" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="36" t="s">
-        <v>96</v>
+      <c r="D20" s="39" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -1497,7 +1474,7 @@
       <c r="C21" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="37"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
@@ -2212,7 +2189,7 @@
         <v>59</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>60</v>
@@ -2788,7 +2765,7 @@
         <v>59</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>65</v>
@@ -3534,16 +3511,16 @@
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="D5" s="22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3557,7 +3534,7 @@
         <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3571,7 +3548,7 @@
         <v>63</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3585,7 +3562,7 @@
         <v>62</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,7 +4270,7 @@
         <v>64</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -4455,7 +4432,7 @@
         <v>64</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>65</v>
@@ -4767,7 +4744,7 @@
         <v>64</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>60</v>
@@ -5271,7 +5248,7 @@
         <v>64</v>
       </c>
       <c r="D1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>65</v>
@@ -5931,19 +5908,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -5996,7 +5973,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -6049,7 +6026,7 @@
         <v>150</v>
       </c>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -6102,7 +6079,7 @@
         <v>-9</v>
       </c>
       <c r="Q4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -6155,7 +6132,7 @@
         <v>-9</v>
       </c>
       <c r="Q5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -6208,7 +6185,7 @@
         <v>-9</v>
       </c>
       <c r="Q6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -6288,19 +6265,19 @@
         <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>85</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>48</v>
@@ -6365,7 +6342,7 @@
         <v>0</v>
       </c>
       <c r="Q2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R2">
         <v>0</v>
@@ -6430,7 +6407,7 @@
         <v>150</v>
       </c>
       <c r="Q3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R3">
         <v>0</v>
@@ -6495,7 +6472,7 @@
         <v>-9</v>
       </c>
       <c r="Q4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R4">
         <v>1</v>
@@ -6560,7 +6537,7 @@
         <v>-9</v>
       </c>
       <c r="Q5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="R5">
         <v>2</v>
@@ -6625,7 +6602,7 @@
         <v>-9</v>
       </c>
       <c r="Q6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="R6" s="2">
         <v>-9</v>
@@ -6650,42 +6627,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D163"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomRight" activeCell="D8" sqref="D8:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" style="53" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" style="53" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="74.7109375" style="53" customWidth="1"/>
-    <col min="4" max="4" width="58" style="48" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="53"/>
+    <col min="1" max="1" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="58" style="12" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="43" t="s">
+      <c r="C1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="36" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -6696,27 +6673,27 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="45" t="s">
+      <c r="A3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="45" t="s">
-        <v>72</v>
-      </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="45" t="s">
+      <c r="A4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -6724,41 +6701,41 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
+      <c r="A5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="45" t="s">
-        <v>99</v>
+      <c r="C5" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="45" t="s">
-        <v>98</v>
+      <c r="D6" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="8" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="3" t="s">
@@ -6769,57 +6746,57 @@
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>49</v>
+      <c r="D8" s="41" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="39"/>
+      <c r="D9" s="42"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="39"/>
+      <c r="D10" s="42"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="43"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -6833,7 +6810,7 @@
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
@@ -6845,13 +6822,13 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B14" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>50</v>
@@ -6859,65 +6836,65 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B15" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B18" s="45" t="s">
+      <c r="C18" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="D18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -6928,74 +6905,74 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="45" t="s">
+      <c r="B20" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="51" t="s">
-        <v>96</v>
+      <c r="D20" s="39" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="52"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
-      <c r="B23" s="48"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="48"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="12"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="48"/>
-      <c r="B25" s="48"/>
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="48"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="48"/>
-      <c r="B27" s="48"/>
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="48"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="48"/>
-      <c r="B29" s="48"/>
+      <c r="A29" s="12"/>
+      <c r="B29" s="12"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="48"/>
-      <c r="B30" s="48"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="48"/>
-      <c r="B32" s="48"/>
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="13"/>
@@ -7034,50 +7011,50 @@
       <c r="D38" s="17"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="48"/>
-      <c r="B39" s="48"/>
+      <c r="A39" s="12"/>
+      <c r="B39" s="12"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="48"/>
-      <c r="B40" s="48"/>
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="48"/>
-      <c r="B41" s="48"/>
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="48"/>
-      <c r="B42" s="48"/>
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="48"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="48"/>
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
+      <c r="A44" s="12"/>
+      <c r="B44" s="12"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
-      <c r="C45" s="48"/>
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
-      <c r="B46" s="48"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="48"/>
-      <c r="B47" s="48"/>
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="48"/>
-      <c r="B48" s="48"/>
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="48"/>
-      <c r="B49" s="48"/>
+      <c r="A49" s="12"/>
+      <c r="B49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="14"/>
@@ -7200,16 +7177,16 @@
       <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="48"/>
-      <c r="B70" s="48"/>
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="48"/>
-      <c r="B71" s="48"/>
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="48"/>
-      <c r="B72" s="48"/>
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="13"/>
@@ -7392,8 +7369,8 @@
       <c r="D102" s="17"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="48"/>
-      <c r="B103" s="48"/>
+      <c r="A103" s="12"/>
+      <c r="B103" s="12"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="13"/>
@@ -7444,116 +7421,116 @@
       <c r="D111" s="15"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="48"/>
-      <c r="B112" s="48"/>
+      <c r="A112" s="12"/>
+      <c r="B112" s="12"/>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="48"/>
-      <c r="B113" s="48"/>
-      <c r="C113" s="48"/>
+      <c r="A113" s="12"/>
+      <c r="B113" s="12"/>
+      <c r="C113" s="12"/>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="48"/>
-      <c r="B114" s="48"/>
-      <c r="C114" s="48"/>
+      <c r="A114" s="12"/>
+      <c r="B114" s="12"/>
+      <c r="C114" s="12"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="48"/>
-      <c r="B115" s="48"/>
-      <c r="C115" s="48"/>
-      <c r="D115" s="53"/>
+      <c r="A115" s="12"/>
+      <c r="B115" s="12"/>
+      <c r="C115" s="12"/>
+      <c r="D115" s="6"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="48"/>
-      <c r="B116" s="48"/>
-      <c r="D116" s="53"/>
+      <c r="A116" s="12"/>
+      <c r="B116" s="12"/>
+      <c r="D116" s="6"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="48"/>
-      <c r="B117" s="48"/>
+      <c r="A117" s="12"/>
+      <c r="B117" s="12"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="48"/>
-      <c r="B118" s="48"/>
-      <c r="D118" s="53"/>
+      <c r="A118" s="12"/>
+      <c r="B118" s="12"/>
+      <c r="D118" s="6"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="48"/>
-      <c r="B119" s="48"/>
-      <c r="D119" s="53"/>
+      <c r="A119" s="12"/>
+      <c r="B119" s="12"/>
+      <c r="D119" s="6"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="48"/>
-      <c r="B120" s="48"/>
+      <c r="A120" s="12"/>
+      <c r="B120" s="12"/>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A121" s="48"/>
-      <c r="B121" s="48"/>
+      <c r="A121" s="12"/>
+      <c r="B121" s="12"/>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="48"/>
-      <c r="B122" s="48"/>
-      <c r="D122" s="53"/>
+      <c r="A122" s="12"/>
+      <c r="B122" s="12"/>
+      <c r="D122" s="6"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="48"/>
-      <c r="B123" s="48"/>
-      <c r="D123" s="53"/>
+      <c r="A123" s="12"/>
+      <c r="B123" s="12"/>
+      <c r="D123" s="6"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="48"/>
-      <c r="B124" s="48"/>
-      <c r="D124" s="53"/>
+      <c r="A124" s="12"/>
+      <c r="B124" s="12"/>
+      <c r="D124" s="6"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="48"/>
-      <c r="B125" s="48"/>
-      <c r="D125" s="53"/>
+      <c r="A125" s="12"/>
+      <c r="B125" s="12"/>
+      <c r="D125" s="6"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D126" s="53"/>
+      <c r="D126" s="6"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D127" s="53"/>
+      <c r="D127" s="6"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D128" s="53"/>
-    </row>
-    <row r="129" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="D128" s="6"/>
+    </row>
+    <row r="129" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="147" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="148" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="149" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="150" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="151" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="152" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="153" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="154" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="155" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="156" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="157" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="158" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="159" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="160" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="161" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="162" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="163" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D20:D21"/>
@@ -7595,321 +7572,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="41" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>73</v>
+      <c r="Q1" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42">
-        <v>0</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0</v>
-      </c>
-      <c r="F2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>-9</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>200</v>
       </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="K2" s="42">
+      <c r="K2">
         <v>60</v>
       </c>
-      <c r="L2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M2" s="42">
-        <v>0</v>
-      </c>
-      <c r="N2" s="42">
-        <v>0</v>
-      </c>
-      <c r="O2" s="42">
-        <v>0</v>
-      </c>
-      <c r="P2" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="42" t="s">
+      <c r="L2">
+        <v>-9</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-9</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>10.55</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+      <c r="K3">
+        <v>-9</v>
+      </c>
+      <c r="L3">
+        <v>-9</v>
+      </c>
+      <c r="M3">
+        <v>25</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-9</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>17.2</v>
+      </c>
+      <c r="G4">
+        <v>-9</v>
+      </c>
+      <c r="H4">
+        <v>-9</v>
+      </c>
+      <c r="I4">
+        <v>-9</v>
+      </c>
+      <c r="J4">
+        <v>-9</v>
+      </c>
+      <c r="K4">
+        <v>-9</v>
+      </c>
+      <c r="L4">
+        <v>-9</v>
+      </c>
+      <c r="M4">
+        <v>-9</v>
+      </c>
+      <c r="N4">
+        <v>-9</v>
+      </c>
+      <c r="O4">
+        <v>-9</v>
+      </c>
+      <c r="P4">
+        <v>-9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-9</v>
+      </c>
+      <c r="G5">
+        <v>-9</v>
+      </c>
+      <c r="H5">
+        <v>-9</v>
+      </c>
+      <c r="I5">
+        <v>-9</v>
+      </c>
+      <c r="J5">
+        <v>-9</v>
+      </c>
+      <c r="K5">
+        <v>-9</v>
+      </c>
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>-9</v>
+      </c>
+      <c r="N5">
+        <v>-9</v>
+      </c>
+      <c r="O5">
+        <v>-9</v>
+      </c>
+      <c r="P5">
+        <v>-9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>-9</v>
+      </c>
+      <c r="D6">
+        <v>-9</v>
+      </c>
+      <c r="E6">
+        <v>-9</v>
+      </c>
+      <c r="F6">
+        <v>-9</v>
+      </c>
+      <c r="G6">
+        <v>-9</v>
+      </c>
+      <c r="H6">
+        <v>-9</v>
+      </c>
+      <c r="I6">
+        <v>-9</v>
+      </c>
+      <c r="J6">
+        <v>-9</v>
+      </c>
+      <c r="K6">
+        <v>-9</v>
+      </c>
+      <c r="L6">
+        <v>-9</v>
+      </c>
+      <c r="M6">
+        <v>-9</v>
+      </c>
+      <c r="N6">
+        <v>-9</v>
+      </c>
+      <c r="O6">
+        <v>-9</v>
+      </c>
+      <c r="P6">
+        <v>-9</v>
+      </c>
+      <c r="Q6" t="s">
         <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
-        <v>2</v>
-      </c>
-      <c r="B3" s="42">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E3" s="42">
-        <v>2</v>
-      </c>
-      <c r="F3" s="42">
-        <v>10.55</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>200</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>200</v>
-      </c>
-      <c r="K3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M3" s="42">
-        <v>25</v>
-      </c>
-      <c r="N3" s="42">
-        <v>30</v>
-      </c>
-      <c r="O3" s="42">
-        <v>20</v>
-      </c>
-      <c r="P3" s="42">
-        <v>150</v>
-      </c>
-      <c r="Q3" s="42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
-        <v>3</v>
-      </c>
-      <c r="B4" s="42">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>2</v>
-      </c>
-      <c r="F4" s="42">
-        <v>17.2</v>
-      </c>
-      <c r="G4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q4" s="42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
-        <v>4</v>
-      </c>
-      <c r="B5" s="42">
-        <v>1</v>
-      </c>
-      <c r="C5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D5" s="42">
-        <v>1</v>
-      </c>
-      <c r="E5" s="42">
-        <v>1</v>
-      </c>
-      <c r="F5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L5" s="42">
-        <v>25</v>
-      </c>
-      <c r="M5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q5" s="42" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
-        <v>5</v>
-      </c>
-      <c r="B6" s="42">
-        <v>2</v>
-      </c>
-      <c r="C6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="F6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -7952,392 +7929,392 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="41" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="41" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="41" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="N1" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q1" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="R1" s="41" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="42">
-        <v>1</v>
-      </c>
-      <c r="B2" s="42">
-        <v>0</v>
-      </c>
-      <c r="C2" s="42">
-        <v>0</v>
-      </c>
-      <c r="D2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E2" s="42">
-        <v>0</v>
-      </c>
-      <c r="F2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G2" s="42">
-        <v>0</v>
-      </c>
-      <c r="H2" s="42">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>-9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>-9</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>200</v>
       </c>
-      <c r="I2" s="42">
-        <v>0</v>
-      </c>
-      <c r="J2" s="42">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>200</v>
       </c>
-      <c r="K2" s="42">
+      <c r="K2">
         <v>60</v>
       </c>
-      <c r="L2" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M2" s="42">
-        <v>0</v>
-      </c>
-      <c r="N2" s="42">
-        <v>0</v>
-      </c>
-      <c r="O2" s="42">
-        <v>0</v>
-      </c>
-      <c r="P2" s="42">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="42" t="s">
+      <c r="L2">
+        <v>-9</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0.1</v>
+      </c>
+      <c r="T2">
+        <v>0.3</v>
+      </c>
+      <c r="U2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-9</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>10.55</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>200</v>
+      </c>
+      <c r="K3">
+        <v>-9</v>
+      </c>
+      <c r="L3">
+        <v>-9</v>
+      </c>
+      <c r="M3">
+        <v>25</v>
+      </c>
+      <c r="N3">
+        <v>30</v>
+      </c>
+      <c r="O3">
+        <v>20</v>
+      </c>
+      <c r="P3">
+        <v>150</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>76</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>-9</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>17.2</v>
+      </c>
+      <c r="G4">
+        <v>-9</v>
+      </c>
+      <c r="H4">
+        <v>-9</v>
+      </c>
+      <c r="I4">
+        <v>-9</v>
+      </c>
+      <c r="J4">
+        <v>-9</v>
+      </c>
+      <c r="K4">
+        <v>-9</v>
+      </c>
+      <c r="L4">
+        <v>-9</v>
+      </c>
+      <c r="M4">
+        <v>-9</v>
+      </c>
+      <c r="N4">
+        <v>-9</v>
+      </c>
+      <c r="O4">
+        <v>-9</v>
+      </c>
+      <c r="P4">
+        <v>-9</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>76</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4">
+        <v>0.2</v>
+      </c>
+      <c r="T4">
+        <v>0.3</v>
+      </c>
+      <c r="U4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>-9</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-9</v>
+      </c>
+      <c r="G5">
+        <v>-9</v>
+      </c>
+      <c r="H5">
+        <v>-9</v>
+      </c>
+      <c r="I5">
+        <v>-9</v>
+      </c>
+      <c r="J5">
+        <v>-9</v>
+      </c>
+      <c r="K5">
+        <v>-9</v>
+      </c>
+      <c r="L5">
+        <v>25</v>
+      </c>
+      <c r="M5">
+        <v>-9</v>
+      </c>
+      <c r="N5">
+        <v>-9</v>
+      </c>
+      <c r="O5">
+        <v>-9</v>
+      </c>
+      <c r="P5">
+        <v>-9</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>76</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="T5">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="U5">
+        <v>0.33400000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>-9</v>
+      </c>
+      <c r="D6">
+        <v>-9</v>
+      </c>
+      <c r="E6">
+        <v>-9</v>
+      </c>
+      <c r="F6">
+        <v>-9</v>
+      </c>
+      <c r="G6">
+        <v>-9</v>
+      </c>
+      <c r="H6">
+        <v>-9</v>
+      </c>
+      <c r="I6">
+        <v>-9</v>
+      </c>
+      <c r="J6">
+        <v>-9</v>
+      </c>
+      <c r="K6">
+        <v>-9</v>
+      </c>
+      <c r="L6">
+        <v>-9</v>
+      </c>
+      <c r="M6">
+        <v>-9</v>
+      </c>
+      <c r="N6">
+        <v>-9</v>
+      </c>
+      <c r="O6">
+        <v>-9</v>
+      </c>
+      <c r="P6">
+        <v>-9</v>
+      </c>
+      <c r="Q6" t="s">
         <v>77</v>
       </c>
-      <c r="R2" s="42">
-        <v>0</v>
-      </c>
-      <c r="S2" s="42">
-        <v>0.1</v>
-      </c>
-      <c r="T2" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="U2" s="42">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="42">
-        <v>2</v>
-      </c>
-      <c r="B3" s="42">
-        <v>0</v>
-      </c>
-      <c r="C3" s="42">
-        <v>1</v>
-      </c>
-      <c r="D3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E3" s="42">
-        <v>2</v>
-      </c>
-      <c r="F3" s="42">
-        <v>10.55</v>
-      </c>
-      <c r="G3" s="42">
-        <v>0</v>
-      </c>
-      <c r="H3" s="42">
-        <v>200</v>
-      </c>
-      <c r="I3" s="42">
-        <v>0</v>
-      </c>
-      <c r="J3" s="42">
-        <v>200</v>
-      </c>
-      <c r="K3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L3" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M3" s="42">
-        <v>25</v>
-      </c>
-      <c r="N3" s="42">
-        <v>30</v>
-      </c>
-      <c r="O3" s="42">
-        <v>20</v>
-      </c>
-      <c r="P3" s="42">
-        <v>150</v>
-      </c>
-      <c r="Q3" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="R3" s="42">
-        <v>0</v>
-      </c>
-      <c r="S3" s="42">
-        <v>1</v>
-      </c>
-      <c r="T3" s="42">
-        <v>0</v>
-      </c>
-      <c r="U3" s="42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="42">
-        <v>3</v>
-      </c>
-      <c r="B4" s="42">
-        <v>1</v>
-      </c>
-      <c r="C4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D4" s="42">
-        <v>0</v>
-      </c>
-      <c r="E4" s="42">
-        <v>2</v>
-      </c>
-      <c r="F4" s="42">
-        <v>17.2</v>
-      </c>
-      <c r="G4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P4" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q4" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="R4" s="42">
-        <v>1</v>
-      </c>
-      <c r="S4" s="42">
-        <v>0.2</v>
-      </c>
-      <c r="T4" s="42">
-        <v>0.3</v>
-      </c>
-      <c r="U4" s="42">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="42">
-        <v>4</v>
-      </c>
-      <c r="B5" s="42">
-        <v>1</v>
-      </c>
-      <c r="C5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D5" s="42">
-        <v>1</v>
-      </c>
-      <c r="E5" s="42">
-        <v>1</v>
-      </c>
-      <c r="F5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L5" s="42">
-        <v>25</v>
-      </c>
-      <c r="M5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P5" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q5" s="42" t="s">
-        <v>77</v>
-      </c>
-      <c r="R5" s="42">
-        <v>2</v>
-      </c>
-      <c r="S5" s="42">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="T5" s="42">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="U5" s="42">
-        <v>0.33400000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="42">
-        <v>5</v>
-      </c>
-      <c r="B6" s="42">
-        <v>2</v>
-      </c>
-      <c r="C6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="D6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="E6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="F6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="G6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="H6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="I6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="J6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="K6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="L6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="M6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="N6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="O6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="P6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>78</v>
-      </c>
-      <c r="R6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="S6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="T6" s="42">
-        <v>-9</v>
-      </c>
-      <c r="U6" s="42">
+      <c r="R6">
+        <v>-9</v>
+      </c>
+      <c r="S6">
+        <v>-9</v>
+      </c>
+      <c r="T6">
+        <v>-9</v>
+      </c>
+      <c r="U6">
         <v>-9</v>
       </c>
     </row>
@@ -8351,12 +8328,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="B2" sqref="B2"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
       <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8420,8 +8397,8 @@
       <c r="C4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>69</v>
+      <c r="D4" s="41" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
@@ -8434,20 +8411,20 @@
       <c r="C5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="43"/>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>94</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8461,7 +8438,7 @@
         <v>67</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8475,7 +8452,7 @@
         <v>63</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8489,7 +8466,7 @@
         <v>62</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9203,7 +9180,7 @@
         <v>59</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -9395,7 +9372,7 @@
         <v>59</v>
       </c>
       <c r="E1" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F1" s="21" t="s">
         <v>65</v>

</xml_diff>